<commit_message>
Initial committ sajjini , Arraypage,DSintro,Basepage,datasheet
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/Data.xlsx
+++ b/src/test/resources/Exceldata/Data.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josephan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F31A5FA-3186-47E7-A2AF-F0AD49AE4A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F566AC6F-F649-4DAF-B999-E7A4A743AD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
+    <sheet name="arrayCode" sheetId="3" r:id="rId3"/>
+    <sheet name="Intro" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>UserName</t>
   </si>
@@ -71,13 +73,117 @@
   </si>
   <si>
     <t>stack page try here</t>
+  </si>
+  <si>
+    <t>print("Hello World")</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t>arraycode</t>
+  </si>
+  <si>
+    <t>introcode</t>
+  </si>
+  <si>
+    <t>NameError:</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 1</t>
+  </si>
+  <si>
+    <t>Element Found</t>
+  </si>
+  <si>
+    <t>submission success</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>def search(list,element):
+    if element in list:
+        return("Element Found")
+    else:
+        return("Not Found")
+li=[9, 2, 34, 2, 5, 9, 16]
+element= 9
+print("Check if",element,"is in",li)
+print(search(li,element))</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):
+    count = 0
+    result = 0
+    for i in range(0, len(nums)):
+        if (nums[i] == 0):
+            count = 0
+        else:
+            count+= 1
+            result = max(result, count)
+    return result
+nums  = [1,0,1,1,0,1]
+n = len(nums)
+print(findMaxConsecutiveOnes(nums))</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+	c=0
+	for i in nums:
+		j=str(i)
+		x=len(j)
+		if x%2==0:
+				c=c+1
+        print (c)
+	return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+	c=0
+	for i in nums:
+		j=str(i)
+		x=len(j)
+		if x%2==0:
+				c=c+1
+	return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+	squares_list = []
+ 	for i in range(0, len(nums)):
+     		square = nums[i] * nums[i];
+     		squares_list.append(square)
+     		sorted_squares_list = sorted(squares_list)
+   	print sorted_squares_list;	
+	return sorted_squares_list; 		
+sortedSquares([-7,-3,2,3,11])</t>
+  </si>
+  <si>
+    <t>No tests were collected</t>
+  </si>
+  <si>
+    <t>def search(list,element):
+    if element in list:
+        return("Element Found")
+    else:
+        return("Not Found")
+li=[9, 2, 34, 2, 5, 9, 16]
+element= 9
+print("Check if",element,"is in",li)
+print(search(li,element))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,13 +199,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -111,17 +240,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{EDF08276-21EE-466A-928B-AEBF83E3871E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -469,9 +608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F62B769-6515-4787-8EF9-279DFE90F425}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -506,4 +643,153 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B9486F-E1C8-4E72-A3C3-9B41E667C831}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6007E19-4637-4E58-9EE0-8A5B26766B33}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
linkedlist and graph features
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/Data.xlsx
+++ b/src/test/resources/Exceldata/Data.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josephan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F31A5FA-3186-47E7-A2AF-F0AD49AE4A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BD9853-1262-4AC1-8C4E-190C352FCE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
+    <sheet name="arrayCode" sheetId="3" r:id="rId3"/>
+    <sheet name="Intro" sheetId="4" r:id="rId4"/>
+    <sheet name="llCode" sheetId="5" r:id="rId5"/>
+    <sheet name="GraphCode" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>UserName</t>
   </si>
@@ -71,13 +75,153 @@
   </si>
   <si>
     <t>stack page try here</t>
+  </si>
+  <si>
+    <t>print("Hello World")</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t>arraycode</t>
+  </si>
+  <si>
+    <t>introcode</t>
+  </si>
+  <si>
+    <t>NameError:</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 1</t>
+  </si>
+  <si>
+    <t>Element Found</t>
+  </si>
+  <si>
+    <t>submission success</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>def search(list,element):
+    if element in list:
+        return("Element Found")
+    else:
+        return("Not Found")
+li=[9, 2, 34, 2, 5, 9, 16]
+element= 9
+print("Check if",element,"is in",li)
+print(search(li,element))</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):
+    count = 0
+    result = 0
+    for i in range(0, len(nums)):
+        if (nums[i] == 0):
+            count = 0
+        else:
+            count+= 1
+            result = max(result, count)
+    return result
+nums  = [1,0,1,1,0,1]
+n = len(nums)
+print(findMaxConsecutiveOnes(nums))</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+	c=0
+	for i in nums:
+		j=str(i)
+		x=len(j)
+		if x%2==0:
+				c=c+1
+        print (c)
+	return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+	c=0
+	for i in nums:
+		j=str(i)
+		x=len(j)
+		if x%2==0:
+				c=c+1
+	return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+	squares_list = []
+ 	for i in range(0, len(nums)):
+     		square = nums[i] * nums[i];
+     		squares_list.append(square)
+     		sorted_squares_list = sorted(squares_list)
+   	print sorted_squares_list;	
+	return sorted_squares_list; 		
+sortedSquares([-7,-3,2,3,11])</t>
+  </si>
+  <si>
+    <t>No tests were collected</t>
+  </si>
+  <si>
+    <t>def search(list,element):
+    if element in list:
+        return("Element Found")
+    else:
+        return("Not Found")
+li=[9, 2, 34, 2, 5, 9, 16]
+element= 9
+print("Check if",element,"is in",li)
+print(search(li,element))</t>
+  </si>
+  <si>
+    <t>print("tree page try here")</t>
+  </si>
+  <si>
+    <t>tree page try here</t>
+  </si>
+  <si>
+    <t>print("queue page try here")</t>
+  </si>
+  <si>
+    <t>queue page try here</t>
+  </si>
+  <si>
+    <t>print("welcome to linkedlist page")</t>
+  </si>
+  <si>
+    <t>welcome to linkedlist page</t>
+  </si>
+  <si>
+    <t>print welcome</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>print("welcome to Graph page")</t>
+  </si>
+  <si>
+    <t>welcome to Graph page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print Graph page </t>
+  </si>
+  <si>
+    <t>Errormsg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,13 +237,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -111,17 +278,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{EDF08276-21EE-466A-928B-AEBF83E3871E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -401,9 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -467,16 +642,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F62B769-6515-4787-8EF9-279DFE90F425}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -503,6 +678,269 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B9486F-E1C8-4E72-A3C3-9B41E667C831}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6007E19-4637-4E58-9EE0-8A5B26766B33}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8FA28C-7A04-47E3-8D86-AA1564B91A6F}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EE4F11-F9C4-46EF-BE41-99F717AEE429}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>